<commit_message>
- add column: BuTruTraHang
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_GiaoDichHoaDon.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_GiaoDichHoaDon.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Tên khách hàng</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>Tỉnh thành</t>
+  </si>
+  <si>
+    <t>Bù trừ trả hàng</t>
+  </si>
+  <si>
+    <t>Giá trị sau trả</t>
   </si>
 </sst>
 </file>
@@ -638,12 +644,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD33"/>
+  <dimension ref="A1:AF33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P1" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,14 +669,16 @@
     <col min="17" max="17" width="13.7109375" style="17" customWidth="1"/>
     <col min="18" max="19" width="18.140625" style="17" customWidth="1"/>
     <col min="20" max="20" width="19.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="19.140625" style="17" customWidth="1"/>
-    <col min="27" max="27" width="18.140625" style="17" customWidth="1"/>
-    <col min="28" max="28" width="18.140625" style="30" customWidth="1"/>
-    <col min="29" max="29" width="21.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="1"/>
+    <col min="21" max="21" width="21.7109375" style="17" customWidth="1"/>
+    <col min="22" max="22" width="20.140625" style="17" customWidth="1"/>
+    <col min="23" max="28" width="19.140625" style="17" customWidth="1"/>
+    <col min="29" max="29" width="18.140625" style="17" customWidth="1"/>
+    <col min="30" max="30" width="18.140625" style="30" customWidth="1"/>
+    <col min="31" max="31" width="21.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>11</v>
       </c>
@@ -702,9 +710,11 @@
       <c r="AA1" s="34"/>
       <c r="AB1" s="34"/>
       <c r="AC1" s="34"/>
-      <c r="AD1" s="4"/>
-    </row>
-    <row r="2" spans="1:30" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="4"/>
+    </row>
+    <row r="2" spans="1:32" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -732,11 +742,13 @@
       <c r="Y2" s="22"/>
       <c r="Z2" s="22"/>
       <c r="AA2" s="22"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="4"/>
-    </row>
-    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="4"/>
+    </row>
+    <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
@@ -766,11 +778,13 @@
       <c r="Y3" s="22"/>
       <c r="Z3" s="22"/>
       <c r="AA3" s="22"/>
-      <c r="AB3" s="26"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="4"/>
-    </row>
-    <row r="4" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="26"/>
+      <c r="AE3" s="26"/>
+      <c r="AF3" s="4"/>
+    </row>
+    <row r="4" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>14</v>
       </c>
@@ -800,11 +814,13 @@
       <c r="Y4" s="22"/>
       <c r="Z4" s="22"/>
       <c r="AA4" s="22"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="4"/>
-    </row>
-    <row r="5" spans="1:30" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="26"/>
+      <c r="AF4" s="4"/>
+    </row>
+    <row r="5" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -832,11 +848,13 @@
       <c r="Y5" s="22"/>
       <c r="Z5" s="22"/>
       <c r="AA5" s="22"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="4"/>
-    </row>
-    <row r="6" spans="1:30" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="4"/>
+    </row>
+    <row r="6" spans="1:32" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -898,34 +916,40 @@
         <v>9</v>
       </c>
       <c r="U6" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="V6" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="W6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="V6" s="24" t="s">
+      <c r="X6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="W6" s="24" t="s">
+      <c r="Y6" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="X6" s="24" t="s">
+      <c r="Z6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="Y6" s="24" t="s">
+      <c r="AA6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="Z6" s="24" t="s">
+      <c r="AB6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="AA6" s="24" t="s">
+      <c r="AC6" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="AB6" s="7" t="s">
+      <c r="AD6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AC6" s="7" t="s">
+      <c r="AE6" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="13"/>
@@ -953,10 +977,12 @@
       <c r="Y7" s="18"/>
       <c r="Z7" s="18"/>
       <c r="AA7" s="18"/>
-      <c r="AB7" s="28"/>
-      <c r="AC7" s="10"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="10"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="13"/>
@@ -984,10 +1010,12 @@
       <c r="Y8" s="18"/>
       <c r="Z8" s="18"/>
       <c r="AA8" s="18"/>
-      <c r="AB8" s="28"/>
-      <c r="AC8" s="10"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="28"/>
+      <c r="AE8" s="10"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="13"/>
@@ -1015,10 +1043,12 @@
       <c r="Y9" s="18"/>
       <c r="Z9" s="18"/>
       <c r="AA9" s="18"/>
-      <c r="AB9" s="28"/>
-      <c r="AC9" s="10"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="28"/>
+      <c r="AE9" s="10"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="13"/>
@@ -1046,10 +1076,12 @@
       <c r="Y10" s="18"/>
       <c r="Z10" s="18"/>
       <c r="AA10" s="18"/>
-      <c r="AB10" s="28"/>
-      <c r="AC10" s="10"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="18"/>
+      <c r="AD10" s="28"/>
+      <c r="AE10" s="10"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="13"/>
@@ -1077,10 +1109,12 @@
       <c r="Y11" s="18"/>
       <c r="Z11" s="18"/>
       <c r="AA11" s="18"/>
-      <c r="AB11" s="28"/>
-      <c r="AC11" s="10"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB11" s="18"/>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="28"/>
+      <c r="AE11" s="10"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="13"/>
@@ -1108,10 +1142,12 @@
       <c r="Y12" s="18"/>
       <c r="Z12" s="18"/>
       <c r="AA12" s="18"/>
-      <c r="AB12" s="28"/>
-      <c r="AC12" s="10"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB12" s="18"/>
+      <c r="AC12" s="18"/>
+      <c r="AD12" s="28"/>
+      <c r="AE12" s="10"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="13"/>
@@ -1139,10 +1175,12 @@
       <c r="Y13" s="18"/>
       <c r="Z13" s="18"/>
       <c r="AA13" s="18"/>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="10"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB13" s="18"/>
+      <c r="AC13" s="18"/>
+      <c r="AD13" s="28"/>
+      <c r="AE13" s="10"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="13"/>
@@ -1170,10 +1208,12 @@
       <c r="Y14" s="18"/>
       <c r="Z14" s="18"/>
       <c r="AA14" s="18"/>
-      <c r="AB14" s="28"/>
-      <c r="AC14" s="10"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB14" s="18"/>
+      <c r="AC14" s="18"/>
+      <c r="AD14" s="28"/>
+      <c r="AE14" s="10"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="13"/>
@@ -1201,10 +1241,12 @@
       <c r="Y15" s="18"/>
       <c r="Z15" s="18"/>
       <c r="AA15" s="18"/>
-      <c r="AB15" s="28"/>
-      <c r="AC15" s="10"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB15" s="18"/>
+      <c r="AC15" s="18"/>
+      <c r="AD15" s="28"/>
+      <c r="AE15" s="10"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="13"/>
@@ -1232,10 +1274,12 @@
       <c r="Y16" s="18"/>
       <c r="Z16" s="18"/>
       <c r="AA16" s="18"/>
-      <c r="AB16" s="28"/>
-      <c r="AC16" s="10"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="28"/>
+      <c r="AE16" s="10"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="13"/>
@@ -1263,10 +1307,12 @@
       <c r="Y17" s="18"/>
       <c r="Z17" s="18"/>
       <c r="AA17" s="18"/>
-      <c r="AB17" s="28"/>
-      <c r="AC17" s="10"/>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB17" s="18"/>
+      <c r="AC17" s="18"/>
+      <c r="AD17" s="28"/>
+      <c r="AE17" s="10"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="13"/>
@@ -1294,10 +1340,12 @@
       <c r="Y18" s="18"/>
       <c r="Z18" s="18"/>
       <c r="AA18" s="18"/>
-      <c r="AB18" s="28"/>
-      <c r="AC18" s="10"/>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB18" s="18"/>
+      <c r="AC18" s="18"/>
+      <c r="AD18" s="28"/>
+      <c r="AE18" s="10"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="13"/>
@@ -1325,10 +1373,12 @@
       <c r="Y19" s="18"/>
       <c r="Z19" s="18"/>
       <c r="AA19" s="18"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="10"/>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB19" s="18"/>
+      <c r="AC19" s="18"/>
+      <c r="AD19" s="28"/>
+      <c r="AE19" s="10"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="13"/>
@@ -1356,10 +1406,12 @@
       <c r="Y20" s="18"/>
       <c r="Z20" s="18"/>
       <c r="AA20" s="18"/>
-      <c r="AB20" s="28"/>
-      <c r="AC20" s="10"/>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB20" s="18"/>
+      <c r="AC20" s="18"/>
+      <c r="AD20" s="28"/>
+      <c r="AE20" s="10"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="13"/>
@@ -1387,10 +1439,12 @@
       <c r="Y21" s="18"/>
       <c r="Z21" s="18"/>
       <c r="AA21" s="18"/>
-      <c r="AB21" s="28"/>
-      <c r="AC21" s="10"/>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB21" s="18"/>
+      <c r="AC21" s="18"/>
+      <c r="AD21" s="28"/>
+      <c r="AE21" s="10"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="13"/>
@@ -1418,10 +1472,12 @@
       <c r="Y22" s="18"/>
       <c r="Z22" s="18"/>
       <c r="AA22" s="18"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="10"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB22" s="18"/>
+      <c r="AC22" s="18"/>
+      <c r="AD22" s="28"/>
+      <c r="AE22" s="10"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="13"/>
@@ -1449,10 +1505,12 @@
       <c r="Y23" s="18"/>
       <c r="Z23" s="18"/>
       <c r="AA23" s="18"/>
-      <c r="AB23" s="28"/>
-      <c r="AC23" s="10"/>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB23" s="18"/>
+      <c r="AC23" s="18"/>
+      <c r="AD23" s="28"/>
+      <c r="AE23" s="10"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="13"/>
@@ -1480,10 +1538,12 @@
       <c r="Y24" s="18"/>
       <c r="Z24" s="18"/>
       <c r="AA24" s="18"/>
-      <c r="AB24" s="28"/>
-      <c r="AC24" s="10"/>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB24" s="18"/>
+      <c r="AC24" s="18"/>
+      <c r="AD24" s="28"/>
+      <c r="AE24" s="10"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="13"/>
@@ -1511,10 +1571,12 @@
       <c r="Y25" s="18"/>
       <c r="Z25" s="18"/>
       <c r="AA25" s="18"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="10"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB25" s="18"/>
+      <c r="AC25" s="18"/>
+      <c r="AD25" s="28"/>
+      <c r="AE25" s="10"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="13"/>
@@ -1542,10 +1604,12 @@
       <c r="Y26" s="18"/>
       <c r="Z26" s="18"/>
       <c r="AA26" s="18"/>
-      <c r="AB26" s="28"/>
-      <c r="AC26" s="10"/>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB26" s="18"/>
+      <c r="AC26" s="18"/>
+      <c r="AD26" s="28"/>
+      <c r="AE26" s="10"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="13"/>
@@ -1573,10 +1637,12 @@
       <c r="Y27" s="18"/>
       <c r="Z27" s="18"/>
       <c r="AA27" s="18"/>
-      <c r="AB27" s="28"/>
-      <c r="AC27" s="10"/>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB27" s="18"/>
+      <c r="AC27" s="18"/>
+      <c r="AD27" s="28"/>
+      <c r="AE27" s="10"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="13"/>
@@ -1604,10 +1670,12 @@
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
-      <c r="AB28" s="28"/>
-      <c r="AC28" s="10"/>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB28" s="18"/>
+      <c r="AC28" s="18"/>
+      <c r="AD28" s="28"/>
+      <c r="AE28" s="10"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="13"/>
@@ -1635,10 +1703,12 @@
       <c r="Y29" s="18"/>
       <c r="Z29" s="18"/>
       <c r="AA29" s="18"/>
-      <c r="AB29" s="28"/>
-      <c r="AC29" s="10"/>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB29" s="18"/>
+      <c r="AC29" s="18"/>
+      <c r="AD29" s="28"/>
+      <c r="AE29" s="10"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="13"/>
@@ -1666,10 +1736,12 @@
       <c r="Y30" s="18"/>
       <c r="Z30" s="18"/>
       <c r="AA30" s="18"/>
-      <c r="AB30" s="28"/>
-      <c r="AC30" s="10"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB30" s="18"/>
+      <c r="AC30" s="18"/>
+      <c r="AD30" s="28"/>
+      <c r="AE30" s="10"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>12</v>
       </c>
@@ -1747,10 +1819,18 @@
         <f xml:space="preserve"> SUM(AA$7:AA30)</f>
         <v>0</v>
       </c>
-      <c r="AB31" s="29"/>
-      <c r="AC31" s="14"/>
-    </row>
-    <row r="33" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AB31" s="25">
+        <f xml:space="preserve"> SUM(AB$7:AB30)</f>
+        <v>0</v>
+      </c>
+      <c r="AC31" s="25">
+        <f xml:space="preserve"> SUM(AC$7:AC30)</f>
+        <v>0</v>
+      </c>
+      <c r="AD31" s="29"/>
+      <c r="AE31" s="14"/>
+    </row>
+    <row r="33" spans="3:31" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1776,13 +1856,15 @@
       <c r="Y33" s="23"/>
       <c r="Z33" s="23"/>
       <c r="AA33" s="23"/>
-      <c r="AB33" s="27"/>
-      <c r="AC33" s="27"/>
+      <c r="AB33" s="23"/>
+      <c r="AC33" s="23"/>
+      <c r="AD33" s="27"/>
+      <c r="AE33" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A1:AC1"/>
+    <mergeCell ref="A1:AE1"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>